<commit_message>
Se agrega calculo de Peng-Robinson
</commit_message>
<xml_diff>
--- a/bot_pfp/resource/datos1569111023.xlsx
+++ b/bot_pfp/resource/datos1569111023.xlsx
@@ -520,22 +520,22 @@
         <v>0.0104</v>
       </c>
       <c r="F2" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8440245546320043</v>
+        <v>0.7111383119035047</v>
       </c>
       <c r="H2" t="n">
-        <v>8708.946995420214</v>
+        <v>9315.118065181918</v>
       </c>
       <c r="I2" t="n">
-        <v>7350.565109123278</v>
+        <v>6624.337336055311</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4790445159039615</v>
+        <v>0.4301448194744298</v>
       </c>
       <c r="L2" t="n">
-        <v>37039.43997737678</v>
+        <v>10530.32048949866</v>
       </c>
     </row>
     <row r="3">
@@ -557,19 +557,19 @@
         <v>0.0979</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G3" t="n">
-        <v>1.10433903927366</v>
+        <v>0.8910542058256088</v>
       </c>
       <c r="H3" t="n">
-        <v>21074.82573175043</v>
+        <v>22541.70222848128</v>
       </c>
       <c r="I3" t="n">
-        <v>23273.75280146108</v>
+        <v>20085.87857715674</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7237464661876856</v>
+        <v>0.6498681911765604</v>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
@@ -580,41 +580,73 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Isobutano</t>
+          <t>Propano</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>58.123</v>
+        <v>44.097</v>
       </c>
       <c r="C4" t="n">
-        <v>527.9</v>
+        <v>616</v>
       </c>
       <c r="D4" t="n">
-        <v>734.46</v>
+        <v>666.0599999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1852</v>
+        <v>0.1522</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G4" t="n">
-        <v>1.337249169546775</v>
+        <v>0.9928385045840092</v>
       </c>
       <c r="H4" t="n">
-        <v>50310.86257824745</v>
+        <v>37926.76834742798</v>
       </c>
       <c r="I4" t="n">
-        <v>67278.1592019433</v>
+        <v>37655.15596976453</v>
       </c>
       <c r="J4" t="n">
-        <v>1.293646428756961</v>
+        <v>0.9027563927797403</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9798859057732061</v>
+        <v>0.6361476736065229</v>
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Heptano Plus</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>237</v>
+      </c>
+      <c r="C5" t="n">
+        <v>563</v>
+      </c>
+      <c r="D5" t="n">
+        <v>916</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.339084988163872</v>
+      </c>
+      <c r="H5" t="n">
+        <v>78484.22924214284</v>
+      </c>
+      <c r="I5" t="n">
+        <v>105097.0531857655</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.358391672383659</v>
+      </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
           <t>A</t>
@@ -623,7 +655,7 @@
     </row>
     <row r="6">
       <c r="L6" t="n">
-        <v>69.58756807080727</v>
+        <v>0.9233872578344503</v>
       </c>
     </row>
     <row r="7">
@@ -635,7 +667,7 @@
     </row>
     <row r="8">
       <c r="L8" t="n">
-        <v>9.187056248084668</v>
+        <v>0.4034974477320561</v>
       </c>
     </row>
     <row r="9">
@@ -647,7 +679,7 @@
     </row>
     <row r="10">
       <c r="L10" t="n">
-        <v>38.69185</v>
+        <v>45.1522</v>
       </c>
     </row>
     <row r="11">
@@ -659,7 +691,7 @@
     </row>
     <row r="12">
       <c r="L12" t="n">
-        <v>9.91846658633462</v>
+        <v>1.070030438770379</v>
       </c>
     </row>
     <row r="13">
@@ -671,7 +703,7 @@
     </row>
     <row r="14">
       <c r="L14" t="n">
-        <v>36.57428335274621</v>
+        <v>26.76490044919463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>